<commit_message>
added cat001 mapping info
</commit_message>
<xml_diff>
--- a/doc/objects/cat001.xlsx
+++ b/doc/objects/cat001.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="398">
   <si>
     <t xml:space="preserve">COLID</t>
   </si>
@@ -1106,6 +1106,9 @@
     <t xml:space="preserve">null in db</t>
   </si>
   <si>
+    <t xml:space="preserve">custom</t>
+  </si>
+  <si>
     <t xml:space="preserve">custom based on 070.Mode-3/A reply</t>
   </si>
   <si>
@@ -1163,7 +1166,7 @@
     <t xml:space="preserve">010.SAC</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO share in frame</t>
+    <t xml:space="preserve">shared in data block</t>
   </si>
   <si>
     <t xml:space="preserve">010.SIC</t>
@@ -1299,7 +1302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1314,6 +1317,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3892,8 +3899,8 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E95" activeCellId="0" sqref="E95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E104" activeCellId="0" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4198,7 +4205,9 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>361</v>
+      </c>
       <c r="B15" s="0" t="s">
         <v>53</v>
       </c>
@@ -4217,7 +4226,7 @@
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>56</v>
@@ -4237,7 +4246,7 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>59</v>
@@ -4249,7 +4258,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>60</v>
@@ -4269,7 +4278,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F18" s="1"/>
       <c r="I18" s="0" t="s">
@@ -4286,8 +4295,8 @@
       <c r="D19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>365</v>
+      <c r="E19" s="6" t="s">
+        <v>366</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>66</v>
@@ -4298,7 +4307,7 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>68</v>
@@ -4316,9 +4325,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>73</v>
@@ -4328,6 +4337,9 @@
       </c>
       <c r="D21" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>355</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>74</v>
@@ -4347,7 +4359,7 @@
         <v>77</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>78</v>
@@ -4423,7 +4435,7 @@
         <v>63</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>90</v>
@@ -4442,8 +4454,8 @@
       <c r="D27" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>368</v>
+      <c r="E27" s="6" t="s">
+        <v>369</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>93</v>
@@ -4463,7 +4475,7 @@
         <v>63</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F28" s="1"/>
       <c r="I28" s="0" t="s">
@@ -4472,7 +4484,7 @@
     </row>
     <row r="29" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>97</v>
@@ -4495,7 +4507,7 @@
     </row>
     <row r="30" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>100</v>
@@ -4688,7 +4700,7 @@
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>133</v>
@@ -4708,7 +4720,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>137</v>
@@ -4748,7 +4760,7 @@
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>143</v>
@@ -4771,7 +4783,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>146</v>
@@ -5035,7 +5047,7 @@
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>187</v>
@@ -5192,7 +5204,7 @@
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>211</v>
@@ -5312,7 +5324,7 @@
         <v>17</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>231</v>
@@ -5332,7 +5344,7 @@
         <v>17</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>234</v>
@@ -5369,6 +5381,9 @@
       <c r="D75" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E75" s="0" t="s">
+        <v>352</v>
+      </c>
       <c r="F75" s="1" t="s">
         <v>241</v>
       </c>
@@ -5387,7 +5402,7 @@
         <v>63</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>244</v>
@@ -5406,8 +5421,8 @@
       <c r="D77" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>378</v>
+      <c r="E77" s="6" t="s">
+        <v>379</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>247</v>
@@ -5426,8 +5441,8 @@
       <c r="D78" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>378</v>
+      <c r="E78" s="6" t="s">
+        <v>379</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>250</v>
@@ -5438,7 +5453,7 @@
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>252</v>
@@ -5450,7 +5465,7 @@
         <v>21</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>253</v>
@@ -5461,7 +5476,7 @@
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>255</v>
@@ -5473,7 +5488,7 @@
         <v>21</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>256</v>
@@ -5493,7 +5508,7 @@
         <v>63</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>259</v>
@@ -5504,7 +5519,7 @@
     </row>
     <row r="82" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>261</v>
@@ -5516,7 +5531,7 @@
         <v>21</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>262</v>
@@ -5527,7 +5542,7 @@
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>264</v>
@@ -5550,7 +5565,7 @@
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>267</v>
@@ -5582,7 +5597,7 @@
         <v>69</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>271</v>
@@ -5610,7 +5625,7 @@
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>277</v>
@@ -5633,7 +5648,7 @@
     </row>
     <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>280</v>
@@ -5668,7 +5683,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>288</v>
@@ -5697,7 +5712,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>293</v>
@@ -5709,7 +5724,7 @@
         <v>12</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>294</v>
@@ -5720,7 +5735,7 @@
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>296</v>
@@ -5743,7 +5758,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>299</v>
@@ -5766,7 +5781,7 @@
     </row>
     <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>302</v>
@@ -5789,7 +5804,7 @@
     </row>
     <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>305</v>
@@ -5801,7 +5816,7 @@
         <v>17</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>306</v>
@@ -5818,7 +5833,7 @@
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>310</v>
@@ -5853,7 +5868,7 @@
         <v>12</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>314</v>
@@ -5864,7 +5879,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>316</v>
@@ -5884,7 +5899,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>319</v>
@@ -5974,7 +5989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
         <v>334</v>
       </c>
@@ -5985,7 +6000,7 @@
         <v>12</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>335</v>
@@ -5994,7 +6009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
         <v>337</v>
       </c>
@@ -6005,7 +6020,7 @@
         <v>12</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>338</v>
@@ -6025,7 +6040,7 @@
         <v>12</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>341</v>

</xml_diff>